<commit_message>
TextAnalyzer y Logo Android
</commit_message>
<xml_diff>
--- a/Documentos del Test/Braindo.xlsx
+++ b/Documentos del Test/Braindo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LuisAlejandro\Documents\GitHub\TesisBraindo\Documentos Psicologo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LuisAlejandro\Documents\GitHub\TesisBraindo\Documentos del Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18683,8 +18683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AZ2" sqref="AZ2"/>
+    <sheetView tabSelected="1" topLeftCell="AG112" workbookViewId="0">
+      <selection activeCell="AV121" sqref="AV121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19485,7 +19485,7 @@
       </c>
       <c r="AX4" s="1"/>
       <c r="BC4" s="17">
-        <f t="shared" ref="BC3:BC66" si="10">(SUM(AS4*$AX$2/100)+(AT4*$AY$2/100)+(AU4*$AZ$2/100)+(AV4*$BA$2/100))</f>
+        <f t="shared" ref="BC4:BC66" si="10">(SUM(AS4*$AX$2/100)+(AT4*$AY$2/100)+(AU4*$AZ$2/100)+(AV4*$BA$2/100))</f>
         <v>15</v>
       </c>
     </row>
@@ -42612,165 +42612,165 @@
     </row>
     <row r="120" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B120" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C120" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D120">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E120" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F120" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G120" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H120">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I120">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J120" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K120" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L120" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M120" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N120">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O120" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P120" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q120" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R120" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S120" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T120" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U120" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V120" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W120" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X120" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y120" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z120">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA120" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB120">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC120" s="9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AD120" s="9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE120" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF120" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG120" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH120" s="9">
         <v>0</v>
       </c>
       <c r="AI120" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ120">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AK120">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AL120">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AM120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN120" s="1">
         <f>(SUM(A120+D120+H120+I120+N120+Z120+AB120))/7</f>
-        <v>0</v>
+        <v>2.7142857142857144</v>
       </c>
       <c r="AO120" s="11">
-        <f t="shared" si="23"/>
-        <v>0</v>
+        <f>(SUM(C120+E120+F120+G120+K120+M120+P120+Q120+R120+U120+X120))/11</f>
+        <v>2.7272727272727271</v>
       </c>
       <c r="AP120" s="11">
-        <f t="shared" si="27"/>
-        <v>0</v>
+        <f>(SUM(B120+J120+L120+O120+S120+T120+V120+W120+AA120+Y120))/10</f>
+        <v>2.7</v>
       </c>
       <c r="AQ120" s="10">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>1.7142857142857142</v>
       </c>
       <c r="AR120">
         <f>SUM(AJ120:AM120)/4</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AS120" s="1">
         <f>AN120/4*100</f>
-        <v>0</v>
+        <v>67.857142857142861</v>
       </c>
       <c r="AT120" s="11">
         <f>AO120/4*100</f>
-        <v>0</v>
+        <v>68.181818181818173</v>
       </c>
       <c r="AU120" s="11">
-        <f t="shared" ref="AU120" si="34">AP120/4*100</f>
-        <v>0</v>
+        <f>AP120/4*100</f>
+        <v>67.5</v>
       </c>
       <c r="AV120" s="10">
-        <f t="shared" ref="AV120" si="35">AQ120/4*100</f>
-        <v>0</v>
+        <f t="shared" ref="AV120" si="34">AQ120/4*100</f>
+        <v>42.857142857142854</v>
       </c>
       <c r="AW120" s="1">
         <f>AR120/4*100</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="BC120" s="18">
         <f>(SUM(AS120*$AX$2/100)+(AT120*$AY$2/100)+(AU120*$AZ$2/100)+(AV120*$BA$2/100))</f>
-        <v>0</v>
+        <v>62.857142857142861</v>
       </c>
     </row>
     <row r="121" spans="1:55" x14ac:dyDescent="0.25">
@@ -42779,7 +42779,7 @@
     <row r="125" spans="1:55" x14ac:dyDescent="0.25">
       <c r="AW125">
         <f>AW120/100</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>